<commit_message>
modify names in tbkeysample
</commit_message>
<xml_diff>
--- a/importer/metadata.xlsx
+++ b/importer/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pilou/dev/platyplus/cerberus/importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969221BD-5258-584C-95C5-CEFB72DD5299}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE7DAC7-9922-1F48-8E20-03DE5B1B3FC3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="14260" xr2:uid="{5441FEBD-B00D-ED43-B1D0-1B0469BA4F3D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5963" uniqueCount="1986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6020" uniqueCount="1999">
   <si>
     <t>Type</t>
   </si>
@@ -5992,6 +5992,45 @@
   </si>
   <si>
     <t>who stage</t>
+  </si>
+  <si>
+    <t>blood pressure diastolic</t>
+  </si>
+  <si>
+    <t>blood pressure systolic</t>
+  </si>
+  <si>
+    <t>sample date</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>amk</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>fq</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -6403,8 +6442,8 @@
   <dimension ref="A1:I1211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A1121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1125" sqref="I1125:I1135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6413,7 +6452,8 @@
     <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="9" width="18.33203125" customWidth="1"/>
+    <col min="6" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -7176,7 +7216,7 @@
       <c r="B32" s="1">
         <v>31</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -7449,7 +7489,7 @@
       <c r="B43" s="1">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -26527,7 +26567,7 @@
       <c r="B879" s="1">
         <v>19</v>
       </c>
-      <c r="C879" s="2" t="s">
+      <c r="C879" s="3" t="s">
         <v>1333</v>
       </c>
       <c r="D879" s="1" t="s">
@@ -26539,7 +26579,9 @@
       <c r="F879" s="1"/>
       <c r="G879" s="1"/>
       <c r="H879" s="1"/>
-      <c r="I879" s="1"/>
+      <c r="I879" s="1" t="s">
+        <v>1987</v>
+      </c>
     </row>
     <row r="880" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A880" t="s">
@@ -26548,7 +26590,7 @@
       <c r="B880" s="1">
         <v>20</v>
       </c>
-      <c r="C880" s="2" t="s">
+      <c r="C880" s="3" t="s">
         <v>1335</v>
       </c>
       <c r="D880" s="1" t="s">
@@ -26560,7 +26602,9 @@
       <c r="F880" s="1"/>
       <c r="G880" s="1"/>
       <c r="H880" s="1"/>
-      <c r="I880" s="1"/>
+      <c r="I880" s="1" t="s">
+        <v>1986</v>
+      </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A881" t="s">
@@ -31115,7 +31159,9 @@
         <v>1823</v>
       </c>
       <c r="H1081" s="1"/>
-      <c r="I1081" s="1"/>
+      <c r="I1081" s="1" t="s">
+        <v>1988</v>
+      </c>
     </row>
     <row r="1082" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1082" t="s">
@@ -31140,7 +31186,9 @@
         <v>1823</v>
       </c>
       <c r="H1082" s="1"/>
-      <c r="I1082" s="1"/>
+      <c r="I1082" s="1" t="s">
+        <v>1989</v>
+      </c>
     </row>
     <row r="1083" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1083" t="s">
@@ -31163,7 +31211,9 @@
         <v>1823</v>
       </c>
       <c r="H1083" s="1"/>
-      <c r="I1083" s="1"/>
+      <c r="I1083" s="1" t="s">
+        <v>1990</v>
+      </c>
     </row>
     <row r="1084" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1084" t="s">
@@ -31186,7 +31236,9 @@
         <v>1823</v>
       </c>
       <c r="H1084" s="1"/>
-      <c r="I1084" s="1"/>
+      <c r="I1084" s="1" t="s">
+        <v>1991</v>
+      </c>
     </row>
     <row r="1085" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1085" t="s">
@@ -31209,7 +31261,9 @@
         <v>1823</v>
       </c>
       <c r="H1085" s="1"/>
-      <c r="I1085" s="1"/>
+      <c r="I1085" s="1" t="s">
+        <v>1992</v>
+      </c>
     </row>
     <row r="1086" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1086" t="s">
@@ -31232,7 +31286,9 @@
         <v>1823</v>
       </c>
       <c r="H1086" s="1"/>
-      <c r="I1086" s="1"/>
+      <c r="I1086" s="1" t="s">
+        <v>1993</v>
+      </c>
     </row>
     <row r="1087" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1087" t="s">
@@ -31255,7 +31311,9 @@
         <v>1823</v>
       </c>
       <c r="H1087" s="1"/>
-      <c r="I1087" s="1"/>
+      <c r="I1087" s="1" t="s">
+        <v>1994</v>
+      </c>
     </row>
     <row r="1088" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1088" t="s">
@@ -31278,7 +31336,9 @@
         <v>1823</v>
       </c>
       <c r="H1088" s="1"/>
-      <c r="I1088" s="1"/>
+      <c r="I1088" s="1" t="s">
+        <v>1995</v>
+      </c>
     </row>
     <row r="1089" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1089" t="s">
@@ -31301,7 +31361,9 @@
         <v>1823</v>
       </c>
       <c r="H1089" s="1"/>
-      <c r="I1089" s="1"/>
+      <c r="I1089" s="1" t="s">
+        <v>1996</v>
+      </c>
     </row>
     <row r="1090" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1090" t="s">
@@ -31324,7 +31386,9 @@
         <v>1823</v>
       </c>
       <c r="H1090" s="1"/>
-      <c r="I1090" s="1"/>
+      <c r="I1090" s="1" t="s">
+        <v>1997</v>
+      </c>
     </row>
     <row r="1091" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1091" t="s">
@@ -31347,7 +31411,9 @@
         <v>1823</v>
       </c>
       <c r="H1091" s="1"/>
-      <c r="I1091" s="1"/>
+      <c r="I1091" s="1" t="s">
+        <v>1998</v>
+      </c>
     </row>
     <row r="1092" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1092" t="s">
@@ -31370,7 +31436,9 @@
         <v>1823</v>
       </c>
       <c r="H1092" s="1"/>
-      <c r="I1092" s="1"/>
+      <c r="I1092" s="1" t="s">
+        <v>1988</v>
+      </c>
     </row>
     <row r="1093" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1093" t="s">
@@ -31395,7 +31463,9 @@
         <v>1823</v>
       </c>
       <c r="H1093" s="1"/>
-      <c r="I1093" s="1"/>
+      <c r="I1093" s="1" t="s">
+        <v>1989</v>
+      </c>
     </row>
     <row r="1094" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1094" t="s">
@@ -31418,7 +31488,9 @@
         <v>1823</v>
       </c>
       <c r="H1094" s="1"/>
-      <c r="I1094" s="1"/>
+      <c r="I1094" s="1" t="s">
+        <v>1990</v>
+      </c>
     </row>
     <row r="1095" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1095" t="s">
@@ -31441,7 +31513,9 @@
         <v>1823</v>
       </c>
       <c r="H1095" s="1"/>
-      <c r="I1095" s="1"/>
+      <c r="I1095" s="1" t="s">
+        <v>1991</v>
+      </c>
     </row>
     <row r="1096" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1096" t="s">
@@ -31464,7 +31538,9 @@
         <v>1823</v>
       </c>
       <c r="H1096" s="1"/>
-      <c r="I1096" s="1"/>
+      <c r="I1096" s="1" t="s">
+        <v>1992</v>
+      </c>
     </row>
     <row r="1097" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1097" t="s">
@@ -31487,7 +31563,9 @@
         <v>1823</v>
       </c>
       <c r="H1097" s="1"/>
-      <c r="I1097" s="1"/>
+      <c r="I1097" s="1" t="s">
+        <v>1993</v>
+      </c>
     </row>
     <row r="1098" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1098" t="s">
@@ -31510,7 +31588,9 @@
         <v>1823</v>
       </c>
       <c r="H1098" s="1"/>
-      <c r="I1098" s="1"/>
+      <c r="I1098" s="1" t="s">
+        <v>1994</v>
+      </c>
     </row>
     <row r="1099" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1099" t="s">
@@ -31533,7 +31613,9 @@
         <v>1823</v>
       </c>
       <c r="H1099" s="1"/>
-      <c r="I1099" s="1"/>
+      <c r="I1099" s="1" t="s">
+        <v>1995</v>
+      </c>
     </row>
     <row r="1100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1100" t="s">
@@ -31556,7 +31638,9 @@
         <v>1823</v>
       </c>
       <c r="H1100" s="1"/>
-      <c r="I1100" s="1"/>
+      <c r="I1100" s="1" t="s">
+        <v>1996</v>
+      </c>
     </row>
     <row r="1101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1101" t="s">
@@ -31579,7 +31663,9 @@
         <v>1823</v>
       </c>
       <c r="H1101" s="1"/>
-      <c r="I1101" s="1"/>
+      <c r="I1101" s="1" t="s">
+        <v>1997</v>
+      </c>
     </row>
     <row r="1102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1102" t="s">
@@ -31602,7 +31688,9 @@
         <v>1823</v>
       </c>
       <c r="H1102" s="1"/>
-      <c r="I1102" s="1"/>
+      <c r="I1102" s="1" t="s">
+        <v>1998</v>
+      </c>
     </row>
     <row r="1103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1103" t="s">
@@ -31625,7 +31713,9 @@
         <v>1823</v>
       </c>
       <c r="H1103" s="1"/>
-      <c r="I1103" s="1"/>
+      <c r="I1103" s="1" t="s">
+        <v>1988</v>
+      </c>
     </row>
     <row r="1104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1104" t="s">
@@ -31650,7 +31740,9 @@
         <v>1823</v>
       </c>
       <c r="H1104" s="1"/>
-      <c r="I1104" s="1"/>
+      <c r="I1104" s="1" t="s">
+        <v>1989</v>
+      </c>
     </row>
     <row r="1105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1105" t="s">
@@ -31673,7 +31765,9 @@
         <v>1823</v>
       </c>
       <c r="H1105" s="1"/>
-      <c r="I1105" s="1"/>
+      <c r="I1105" s="1" t="s">
+        <v>1990</v>
+      </c>
     </row>
     <row r="1106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1106" t="s">
@@ -31696,7 +31790,9 @@
         <v>1823</v>
       </c>
       <c r="H1106" s="1"/>
-      <c r="I1106" s="1"/>
+      <c r="I1106" s="1" t="s">
+        <v>1991</v>
+      </c>
     </row>
     <row r="1107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1107" t="s">
@@ -31719,7 +31815,9 @@
         <v>1823</v>
       </c>
       <c r="H1107" s="1"/>
-      <c r="I1107" s="1"/>
+      <c r="I1107" s="1" t="s">
+        <v>1992</v>
+      </c>
     </row>
     <row r="1108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1108" t="s">
@@ -31742,7 +31840,9 @@
         <v>1823</v>
       </c>
       <c r="H1108" s="1"/>
-      <c r="I1108" s="1"/>
+      <c r="I1108" s="1" t="s">
+        <v>1993</v>
+      </c>
     </row>
     <row r="1109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1109" t="s">
@@ -31765,7 +31865,9 @@
         <v>1823</v>
       </c>
       <c r="H1109" s="1"/>
-      <c r="I1109" s="1"/>
+      <c r="I1109" s="1" t="s">
+        <v>1994</v>
+      </c>
     </row>
     <row r="1110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1110" t="s">
@@ -31788,7 +31890,9 @@
         <v>1823</v>
       </c>
       <c r="H1110" s="1"/>
-      <c r="I1110" s="1"/>
+      <c r="I1110" s="1" t="s">
+        <v>1995</v>
+      </c>
     </row>
     <row r="1111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1111" t="s">
@@ -31811,7 +31915,9 @@
         <v>1823</v>
       </c>
       <c r="H1111" s="1"/>
-      <c r="I1111" s="1"/>
+      <c r="I1111" s="1" t="s">
+        <v>1996</v>
+      </c>
     </row>
     <row r="1112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1112" t="s">
@@ -31834,7 +31940,9 @@
         <v>1823</v>
       </c>
       <c r="H1112" s="1"/>
-      <c r="I1112" s="1"/>
+      <c r="I1112" s="1" t="s">
+        <v>1997</v>
+      </c>
     </row>
     <row r="1113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1113" t="s">
@@ -31857,7 +31965,9 @@
         <v>1823</v>
       </c>
       <c r="H1113" s="1"/>
-      <c r="I1113" s="1"/>
+      <c r="I1113" s="1" t="s">
+        <v>1998</v>
+      </c>
     </row>
     <row r="1114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1114" t="s">
@@ -31880,7 +31990,9 @@
         <v>1823</v>
       </c>
       <c r="H1114" s="1"/>
-      <c r="I1114" s="1"/>
+      <c r="I1114" s="1" t="s">
+        <v>1988</v>
+      </c>
     </row>
     <row r="1115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1115" t="s">
@@ -31905,7 +32017,9 @@
         <v>1823</v>
       </c>
       <c r="H1115" s="1"/>
-      <c r="I1115" s="1"/>
+      <c r="I1115" s="1" t="s">
+        <v>1989</v>
+      </c>
     </row>
     <row r="1116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1116" t="s">
@@ -31928,7 +32042,9 @@
         <v>1823</v>
       </c>
       <c r="H1116" s="1"/>
-      <c r="I1116" s="1"/>
+      <c r="I1116" s="1" t="s">
+        <v>1990</v>
+      </c>
     </row>
     <row r="1117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1117" t="s">
@@ -31951,7 +32067,9 @@
         <v>1823</v>
       </c>
       <c r="H1117" s="1"/>
-      <c r="I1117" s="1"/>
+      <c r="I1117" s="1" t="s">
+        <v>1991</v>
+      </c>
     </row>
     <row r="1118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1118" t="s">
@@ -31974,7 +32092,9 @@
         <v>1823</v>
       </c>
       <c r="H1118" s="1"/>
-      <c r="I1118" s="1"/>
+      <c r="I1118" s="1" t="s">
+        <v>1992</v>
+      </c>
     </row>
     <row r="1119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1119" t="s">
@@ -31997,7 +32117,9 @@
         <v>1823</v>
       </c>
       <c r="H1119" s="1"/>
-      <c r="I1119" s="1"/>
+      <c r="I1119" s="1" t="s">
+        <v>1993</v>
+      </c>
     </row>
     <row r="1120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1120" t="s">
@@ -32020,7 +32142,9 @@
         <v>1823</v>
       </c>
       <c r="H1120" s="1"/>
-      <c r="I1120" s="1"/>
+      <c r="I1120" s="1" t="s">
+        <v>1994</v>
+      </c>
     </row>
     <row r="1121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1121" t="s">
@@ -32043,7 +32167,9 @@
         <v>1823</v>
       </c>
       <c r="H1121" s="1"/>
-      <c r="I1121" s="1"/>
+      <c r="I1121" s="1" t="s">
+        <v>1995</v>
+      </c>
     </row>
     <row r="1122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1122" t="s">
@@ -32066,7 +32192,9 @@
         <v>1823</v>
       </c>
       <c r="H1122" s="1"/>
-      <c r="I1122" s="1"/>
+      <c r="I1122" s="1" t="s">
+        <v>1996</v>
+      </c>
     </row>
     <row r="1123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1123" t="s">
@@ -32089,7 +32217,9 @@
         <v>1823</v>
       </c>
       <c r="H1123" s="1"/>
-      <c r="I1123" s="1"/>
+      <c r="I1123" s="1" t="s">
+        <v>1997</v>
+      </c>
     </row>
     <row r="1124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1124" t="s">
@@ -32112,7 +32242,9 @@
         <v>1823</v>
       </c>
       <c r="H1124" s="1"/>
-      <c r="I1124" s="1"/>
+      <c r="I1124" s="1" t="s">
+        <v>1998</v>
+      </c>
     </row>
     <row r="1125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1125" t="s">
@@ -32135,7 +32267,9 @@
         <v>1823</v>
       </c>
       <c r="H1125" s="1"/>
-      <c r="I1125" s="1"/>
+      <c r="I1125" s="1" t="s">
+        <v>1988</v>
+      </c>
     </row>
     <row r="1126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1126" t="s">
@@ -32160,7 +32294,9 @@
         <v>1823</v>
       </c>
       <c r="H1126" s="1"/>
-      <c r="I1126" s="1"/>
+      <c r="I1126" s="1" t="s">
+        <v>1989</v>
+      </c>
     </row>
     <row r="1127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1127" t="s">
@@ -32183,7 +32319,9 @@
         <v>1823</v>
       </c>
       <c r="H1127" s="1"/>
-      <c r="I1127" s="1"/>
+      <c r="I1127" s="1" t="s">
+        <v>1990</v>
+      </c>
     </row>
     <row r="1128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1128" t="s">
@@ -32206,7 +32344,9 @@
         <v>1823</v>
       </c>
       <c r="H1128" s="1"/>
-      <c r="I1128" s="1"/>
+      <c r="I1128" s="1" t="s">
+        <v>1991</v>
+      </c>
     </row>
     <row r="1129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1129" t="s">
@@ -32229,7 +32369,9 @@
         <v>1823</v>
       </c>
       <c r="H1129" s="1"/>
-      <c r="I1129" s="1"/>
+      <c r="I1129" s="1" t="s">
+        <v>1992</v>
+      </c>
     </row>
     <row r="1130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1130" t="s">
@@ -32252,7 +32394,9 @@
         <v>1823</v>
       </c>
       <c r="H1130" s="1"/>
-      <c r="I1130" s="1"/>
+      <c r="I1130" s="1" t="s">
+        <v>1993</v>
+      </c>
     </row>
     <row r="1131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1131" t="s">
@@ -32275,7 +32419,9 @@
         <v>1823</v>
       </c>
       <c r="H1131" s="1"/>
-      <c r="I1131" s="1"/>
+      <c r="I1131" s="1" t="s">
+        <v>1994</v>
+      </c>
     </row>
     <row r="1132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1132" t="s">
@@ -32298,7 +32444,9 @@
         <v>1823</v>
       </c>
       <c r="H1132" s="1"/>
-      <c r="I1132" s="1"/>
+      <c r="I1132" s="1" t="s">
+        <v>1995</v>
+      </c>
     </row>
     <row r="1133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1133" t="s">
@@ -32321,7 +32469,9 @@
         <v>1823</v>
       </c>
       <c r="H1133" s="1"/>
-      <c r="I1133" s="1"/>
+      <c r="I1133" s="1" t="s">
+        <v>1996</v>
+      </c>
     </row>
     <row r="1134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1134" t="s">
@@ -32344,7 +32494,9 @@
         <v>1823</v>
       </c>
       <c r="H1134" s="1"/>
-      <c r="I1134" s="1"/>
+      <c r="I1134" s="1" t="s">
+        <v>1997</v>
+      </c>
     </row>
     <row r="1135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1135" t="s">
@@ -32367,7 +32519,9 @@
         <v>1823</v>
       </c>
       <c r="H1135" s="1"/>
-      <c r="I1135" s="1"/>
+      <c r="I1135" s="1" t="s">
+        <v>1998</v>
+      </c>
     </row>
     <row r="1136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1136" t="s">

</xml_diff>

<commit_message>
typo in the metadata
</commit_message>
<xml_diff>
--- a/importer/metadata.xlsx
+++ b/importer/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pilou/dev/platyplus/cerberus/importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B5EBE9-04FE-1E45-91DD-5BABFBB0B1D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB02DB44-73E6-E242-99FF-BCAA0BA6637F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="14260" xr2:uid="{5441FEBD-B00D-ED43-B1D0-1B0469BA4F3D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10550" uniqueCount="3840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10550" uniqueCount="3839">
   <si>
     <t>Type</t>
   </si>
@@ -11404,9 +11404,6 @@
   </si>
   <si>
     <t>recreational; other</t>
-  </si>
-  <si>
-    <t>DrugType</t>
   </si>
   <si>
     <t>alcohol</t>
@@ -12053,8 +12050,8 @@
   <dimension ref="A1:N1511"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L114" sqref="L114:L117"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15078,17 +15075,17 @@
         <v>2366</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>3790</v>
+        <v>3834</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M90" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15116,17 +15113,17 @@
         <v>2367</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M91" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15154,17 +15151,17 @@
         <v>2368</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M92" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15192,17 +15189,17 @@
         <v>2369</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M93" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15230,17 +15227,17 @@
         <v>2370</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I94" s="2"/>
       <c r="J94" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M94" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15268,17 +15265,17 @@
         <v>2371</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M95" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15306,17 +15303,17 @@
         <v>2372</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M96" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15344,17 +15341,17 @@
         <v>2373</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M97" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15382,17 +15379,17 @@
         <v>2374</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I98" s="2"/>
       <c r="J98" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M98" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15420,17 +15417,17 @@
         <v>2375</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M99" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15458,17 +15455,17 @@
         <v>2376</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I100" s="2"/>
       <c r="J100" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M100" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15496,17 +15493,17 @@
         <v>2377</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I101" s="2"/>
       <c r="J101" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M101" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15534,17 +15531,17 @@
         <v>2378</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M102" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15572,17 +15569,17 @@
         <v>2379</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M103" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15610,17 +15607,17 @@
         <v>2380</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M104" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15648,17 +15645,17 @@
         <v>2381</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M105" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15686,17 +15683,17 @@
         <v>2382</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M106" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15724,17 +15721,17 @@
         <v>2383</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M107" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15762,17 +15759,17 @@
         <v>2384</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I108" s="2"/>
       <c r="J108" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M108" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15800,17 +15797,17 @@
         <v>2385</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I109" s="2"/>
       <c r="J109" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M109" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15838,17 +15835,17 @@
         <v>2386</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I110" s="2"/>
       <c r="J110" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M110" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15876,17 +15873,17 @@
         <v>2387</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I111" s="2"/>
       <c r="J111" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M111" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15914,17 +15911,17 @@
         <v>2388</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I112" s="2"/>
       <c r="J112" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M112" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15952,17 +15949,17 @@
         <v>2389</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I113" s="2"/>
       <c r="J113" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M113" s="26" t="str">
         <f t="shared" si="1"/>
@@ -15990,17 +15987,17 @@
         <v>2390</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I114" s="2"/>
       <c r="J114" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="M114" s="26" t="str">
         <f t="shared" si="1"/>
@@ -16028,17 +16025,17 @@
         <v>2391</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I115" s="2"/>
       <c r="J115" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="M115" s="26" t="str">
         <f t="shared" si="1"/>
@@ -16066,17 +16063,17 @@
         <v>2392</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I116" s="2"/>
       <c r="J116" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="M116" s="26" t="str">
         <f t="shared" si="1"/>
@@ -16104,17 +16101,17 @@
         <v>2393</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="I117" s="2"/>
       <c r="J117" s="2" t="s">
         <v>1899</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
       <c r="L117" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="M117" s="26" t="str">
         <f t="shared" si="1"/>
@@ -20654,14 +20651,14 @@
         <v>2522</v>
       </c>
       <c r="H254" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I254" s="2"/>
       <c r="J254" s="2" t="s">
+        <v>3798</v>
+      </c>
+      <c r="K254" s="2" t="s">
         <v>3799</v>
-      </c>
-      <c r="K254" s="2" t="s">
-        <v>3800</v>
       </c>
       <c r="L254" s="2" t="s">
         <v>1917</v>
@@ -20694,14 +20691,14 @@
         <v>2523</v>
       </c>
       <c r="H255" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I255" s="2"/>
       <c r="J255" s="2" t="s">
+        <v>3798</v>
+      </c>
+      <c r="K255" s="2" t="s">
         <v>3799</v>
-      </c>
-      <c r="K255" s="2" t="s">
-        <v>3800</v>
       </c>
       <c r="L255" s="2" t="s">
         <v>1918</v>
@@ -20734,14 +20731,14 @@
         <v>2524</v>
       </c>
       <c r="H256" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I256" s="2"/>
       <c r="J256" s="2" t="s">
+        <v>3798</v>
+      </c>
+      <c r="K256" s="2" t="s">
         <v>3799</v>
-      </c>
-      <c r="K256" s="2" t="s">
-        <v>3800</v>
       </c>
       <c r="L256" s="2" t="s">
         <v>1919</v>
@@ -20774,14 +20771,14 @@
         <v>2525</v>
       </c>
       <c r="H257" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I257" s="2"/>
       <c r="J257" s="2" t="s">
+        <v>3798</v>
+      </c>
+      <c r="K257" s="2" t="s">
         <v>3799</v>
-      </c>
-      <c r="K257" s="2" t="s">
-        <v>3800</v>
       </c>
       <c r="L257" s="2" t="s">
         <v>1920</v>
@@ -20814,14 +20811,14 @@
         <v>2526</v>
       </c>
       <c r="H258" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I258" s="2"/>
       <c r="J258" s="2" t="s">
+        <v>3798</v>
+      </c>
+      <c r="K258" s="2" t="s">
         <v>3799</v>
-      </c>
-      <c r="K258" s="2" t="s">
-        <v>3800</v>
       </c>
       <c r="L258" s="2" t="s">
         <v>1921</v>
@@ -20854,14 +20851,14 @@
         <v>2527</v>
       </c>
       <c r="H259" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I259" s="2"/>
       <c r="J259" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="K259" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="L259" s="2" t="s">
         <v>1917</v>
@@ -20894,14 +20891,14 @@
         <v>2528</v>
       </c>
       <c r="H260" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I260" s="2"/>
       <c r="J260" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="K260" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="L260" s="2" t="s">
         <v>1918</v>
@@ -20934,14 +20931,14 @@
         <v>2529</v>
       </c>
       <c r="H261" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I261" s="2"/>
       <c r="J261" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="K261" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="L261" s="2" t="s">
         <v>1919</v>
@@ -20974,14 +20971,14 @@
         <v>2530</v>
       </c>
       <c r="H262" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I262" s="2"/>
       <c r="J262" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="K262" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="L262" s="2" t="s">
         <v>1920</v>
@@ -21014,14 +21011,14 @@
         <v>2531</v>
       </c>
       <c r="H263" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="I263" s="2"/>
       <c r="J263" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="K263" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="L263" s="2" t="s">
         <v>1921</v>
@@ -27582,7 +27579,7 @@
       <c r="J458" s="2"/>
       <c r="K458" s="2"/>
       <c r="L458" s="2" t="s">
-        <v>3817</v>
+        <v>3816</v>
       </c>
       <c r="M458" s="26" t="str">
         <f t="shared" si="7"/>
@@ -27744,7 +27741,7 @@
       <c r="J463" s="2"/>
       <c r="K463" s="2"/>
       <c r="L463" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M463" s="26" t="str">
         <f t="shared" si="7"/>
@@ -27812,7 +27809,7 @@
       <c r="J465" s="2"/>
       <c r="K465" s="2"/>
       <c r="L465" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M465" s="26" t="str">
         <f t="shared" si="7"/>
@@ -27846,7 +27843,7 @@
       <c r="J466" s="2"/>
       <c r="K466" s="2"/>
       <c r="L466" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M466" s="26" t="str">
         <f t="shared" si="7"/>
@@ -27914,7 +27911,7 @@
       <c r="J468" s="2"/>
       <c r="K468" s="2"/>
       <c r="L468" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M468" s="26" t="str">
         <f t="shared" si="7"/>
@@ -27948,7 +27945,7 @@
       <c r="J469" s="2"/>
       <c r="K469" s="2"/>
       <c r="L469" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M469" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28016,7 +28013,7 @@
       <c r="J471" s="2"/>
       <c r="K471" s="2"/>
       <c r="L471" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M471" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28050,7 +28047,7 @@
       <c r="J472" s="2"/>
       <c r="K472" s="2"/>
       <c r="L472" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M472" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28118,7 +28115,7 @@
       <c r="J474" s="2"/>
       <c r="K474" s="2"/>
       <c r="L474" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M474" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28152,7 +28149,7 @@
       <c r="J475" s="2"/>
       <c r="K475" s="2"/>
       <c r="L475" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M475" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28220,7 +28217,7 @@
       <c r="J477" s="2"/>
       <c r="K477" s="2"/>
       <c r="L477" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M477" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28254,7 +28251,7 @@
       <c r="J478" s="2"/>
       <c r="K478" s="2"/>
       <c r="L478" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M478" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28322,7 +28319,7 @@
       <c r="J480" s="2"/>
       <c r="K480" s="2"/>
       <c r="L480" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M480" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28356,7 +28353,7 @@
       <c r="J481" s="2"/>
       <c r="K481" s="2"/>
       <c r="L481" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M481" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28424,7 +28421,7 @@
       <c r="J483" s="2"/>
       <c r="K483" s="2"/>
       <c r="L483" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M483" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28458,7 +28455,7 @@
       <c r="J484" s="2"/>
       <c r="K484" s="2"/>
       <c r="L484" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M484" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28526,7 +28523,7 @@
       <c r="J486" s="2"/>
       <c r="K486" s="2"/>
       <c r="L486" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M486" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28560,7 +28557,7 @@
       <c r="J487" s="2"/>
       <c r="K487" s="2"/>
       <c r="L487" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M487" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28628,7 +28625,7 @@
       <c r="J489" s="2"/>
       <c r="K489" s="2"/>
       <c r="L489" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M489" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28662,7 +28659,7 @@
       <c r="J490" s="2"/>
       <c r="K490" s="2"/>
       <c r="L490" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M490" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28730,7 +28727,7 @@
       <c r="J492" s="2"/>
       <c r="K492" s="2"/>
       <c r="L492" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M492" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28764,7 +28761,7 @@
       <c r="J493" s="2"/>
       <c r="K493" s="2"/>
       <c r="L493" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M493" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28832,7 +28829,7 @@
       <c r="J495" s="2"/>
       <c r="K495" s="2"/>
       <c r="L495" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M495" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28866,7 +28863,7 @@
       <c r="J496" s="2"/>
       <c r="K496" s="2"/>
       <c r="L496" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M496" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28934,7 +28931,7 @@
       <c r="J498" s="2"/>
       <c r="K498" s="2"/>
       <c r="L498" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M498" s="26" t="str">
         <f t="shared" si="7"/>
@@ -28968,7 +28965,7 @@
       <c r="J499" s="2"/>
       <c r="K499" s="2"/>
       <c r="L499" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M499" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29036,7 +29033,7 @@
       <c r="J501" s="2"/>
       <c r="K501" s="2"/>
       <c r="L501" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M501" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29070,7 +29067,7 @@
       <c r="J502" s="2"/>
       <c r="K502" s="2"/>
       <c r="L502" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M502" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29138,7 +29135,7 @@
       <c r="J504" s="2"/>
       <c r="K504" s="2"/>
       <c r="L504" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M504" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29172,7 +29169,7 @@
       <c r="J505" s="2"/>
       <c r="K505" s="2"/>
       <c r="L505" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M505" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29240,7 +29237,7 @@
       <c r="J507" s="2"/>
       <c r="K507" s="2"/>
       <c r="L507" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M507" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29274,7 +29271,7 @@
       <c r="J508" s="2"/>
       <c r="K508" s="2"/>
       <c r="L508" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M508" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29342,7 +29339,7 @@
       <c r="J510" s="2"/>
       <c r="K510" s="2"/>
       <c r="L510" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M510" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29376,7 +29373,7 @@
       <c r="J511" s="2"/>
       <c r="K511" s="2"/>
       <c r="L511" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M511" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29444,7 +29441,7 @@
       <c r="J513" s="2"/>
       <c r="K513" s="2"/>
       <c r="L513" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M513" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29478,7 +29475,7 @@
       <c r="J514" s="2"/>
       <c r="K514" s="2"/>
       <c r="L514" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M514" s="26" t="str">
         <f t="shared" si="7"/>
@@ -29546,7 +29543,7 @@
       <c r="J516" s="2"/>
       <c r="K516" s="2"/>
       <c r="L516" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M516" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29580,7 +29577,7 @@
       <c r="J517" s="2"/>
       <c r="K517" s="2"/>
       <c r="L517" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M517" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29648,7 +29645,7 @@
       <c r="J519" s="2"/>
       <c r="K519" s="2"/>
       <c r="L519" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M519" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29682,7 +29679,7 @@
       <c r="J520" s="2"/>
       <c r="K520" s="2"/>
       <c r="L520" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M520" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29750,7 +29747,7 @@
       <c r="J522" s="2"/>
       <c r="K522" s="2"/>
       <c r="L522" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M522" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29784,7 +29781,7 @@
       <c r="J523" s="2"/>
       <c r="K523" s="2"/>
       <c r="L523" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M523" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29852,7 +29849,7 @@
       <c r="J525" s="2"/>
       <c r="K525" s="2"/>
       <c r="L525" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M525" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29886,7 +29883,7 @@
       <c r="J526" s="2"/>
       <c r="K526" s="2"/>
       <c r="L526" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M526" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29954,7 +29951,7 @@
       <c r="J528" s="2"/>
       <c r="K528" s="2"/>
       <c r="L528" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M528" s="26" t="str">
         <f t="shared" si="8"/>
@@ -29988,7 +29985,7 @@
       <c r="J529" s="2"/>
       <c r="K529" s="2"/>
       <c r="L529" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M529" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30056,7 +30053,7 @@
       <c r="J531" s="2"/>
       <c r="K531" s="2"/>
       <c r="L531" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M531" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30090,7 +30087,7 @@
       <c r="J532" s="2"/>
       <c r="K532" s="2"/>
       <c r="L532" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M532" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30158,7 +30155,7 @@
       <c r="J534" s="2"/>
       <c r="K534" s="2"/>
       <c r="L534" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M534" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30192,7 +30189,7 @@
       <c r="J535" s="2"/>
       <c r="K535" s="2"/>
       <c r="L535" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M535" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30260,7 +30257,7 @@
       <c r="J537" s="2"/>
       <c r="K537" s="2"/>
       <c r="L537" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M537" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30294,7 +30291,7 @@
       <c r="J538" s="2"/>
       <c r="K538" s="2"/>
       <c r="L538" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M538" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30362,7 +30359,7 @@
       <c r="J540" s="2"/>
       <c r="K540" s="2"/>
       <c r="L540" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M540" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30396,7 +30393,7 @@
       <c r="J541" s="2"/>
       <c r="K541" s="2"/>
       <c r="L541" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M541" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30464,7 +30461,7 @@
       <c r="J543" s="2"/>
       <c r="K543" s="2"/>
       <c r="L543" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M543" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30498,7 +30495,7 @@
       <c r="J544" s="2"/>
       <c r="K544" s="2"/>
       <c r="L544" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M544" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30566,7 +30563,7 @@
       <c r="J546" s="2"/>
       <c r="K546" s="2"/>
       <c r="L546" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M546" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30600,7 +30597,7 @@
       <c r="J547" s="2"/>
       <c r="K547" s="2"/>
       <c r="L547" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M547" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30668,7 +30665,7 @@
       <c r="J549" s="2"/>
       <c r="K549" s="2"/>
       <c r="L549" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M549" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30702,7 +30699,7 @@
       <c r="J550" s="2"/>
       <c r="K550" s="2"/>
       <c r="L550" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M550" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30770,7 +30767,7 @@
       <c r="J552" s="2"/>
       <c r="K552" s="2"/>
       <c r="L552" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M552" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30804,7 +30801,7 @@
       <c r="J553" s="2"/>
       <c r="K553" s="2"/>
       <c r="L553" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M553" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30872,7 +30869,7 @@
       <c r="J555" s="2"/>
       <c r="K555" s="2"/>
       <c r="L555" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M555" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30906,7 +30903,7 @@
       <c r="J556" s="2"/>
       <c r="K556" s="2"/>
       <c r="L556" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M556" s="26" t="str">
         <f t="shared" si="8"/>
@@ -30974,7 +30971,7 @@
       <c r="J558" s="2"/>
       <c r="K558" s="2"/>
       <c r="L558" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M558" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31008,7 +31005,7 @@
       <c r="J559" s="2"/>
       <c r="K559" s="2"/>
       <c r="L559" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M559" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31076,7 +31073,7 @@
       <c r="J561" s="2"/>
       <c r="K561" s="2"/>
       <c r="L561" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M561" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31110,7 +31107,7 @@
       <c r="J562" s="2"/>
       <c r="K562" s="2"/>
       <c r="L562" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M562" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31178,7 +31175,7 @@
       <c r="J564" s="2"/>
       <c r="K564" s="2"/>
       <c r="L564" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M564" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31212,7 +31209,7 @@
       <c r="J565" s="2"/>
       <c r="K565" s="2"/>
       <c r="L565" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M565" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31280,7 +31277,7 @@
       <c r="J567" s="2"/>
       <c r="K567" s="2"/>
       <c r="L567" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M567" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31314,7 +31311,7 @@
       <c r="J568" s="2"/>
       <c r="K568" s="2"/>
       <c r="L568" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M568" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31382,7 +31379,7 @@
       <c r="J570" s="2"/>
       <c r="K570" s="2"/>
       <c r="L570" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M570" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31416,7 +31413,7 @@
       <c r="J571" s="2"/>
       <c r="K571" s="2"/>
       <c r="L571" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M571" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31484,7 +31481,7 @@
       <c r="J573" s="2"/>
       <c r="K573" s="2"/>
       <c r="L573" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M573" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31518,7 +31515,7 @@
       <c r="J574" s="2"/>
       <c r="K574" s="2"/>
       <c r="L574" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M574" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31586,7 +31583,7 @@
       <c r="J576" s="2"/>
       <c r="K576" s="2"/>
       <c r="L576" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M576" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31620,7 +31617,7 @@
       <c r="J577" s="2"/>
       <c r="K577" s="2"/>
       <c r="L577" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M577" s="26" t="str">
         <f t="shared" si="8"/>
@@ -31688,7 +31685,7 @@
       <c r="J579" s="2"/>
       <c r="K579" s="2"/>
       <c r="L579" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M579" s="26" t="str">
         <f t="shared" ref="M579:M642" si="9">IF(C579="Numeric", "number",IF(C579="Date","date",IF(E579="Yes ; No", "boolean","string")))</f>
@@ -31722,7 +31719,7 @@
       <c r="J580" s="2"/>
       <c r="K580" s="2"/>
       <c r="L580" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M580" s="26" t="str">
         <f t="shared" si="9"/>
@@ -31790,7 +31787,7 @@
       <c r="J582" s="2"/>
       <c r="K582" s="2"/>
       <c r="L582" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M582" s="26" t="str">
         <f t="shared" si="9"/>
@@ -31824,7 +31821,7 @@
       <c r="J583" s="2"/>
       <c r="K583" s="2"/>
       <c r="L583" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M583" s="26" t="str">
         <f t="shared" si="9"/>
@@ -31892,7 +31889,7 @@
       <c r="J585" s="2"/>
       <c r="K585" s="2"/>
       <c r="L585" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M585" s="26" t="str">
         <f t="shared" si="9"/>
@@ -31926,7 +31923,7 @@
       <c r="J586" s="2"/>
       <c r="K586" s="2"/>
       <c r="L586" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M586" s="26" t="str">
         <f t="shared" si="9"/>
@@ -31994,7 +31991,7 @@
       <c r="J588" s="2"/>
       <c r="K588" s="2"/>
       <c r="L588" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M588" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32028,7 +32025,7 @@
       <c r="J589" s="2"/>
       <c r="K589" s="2"/>
       <c r="L589" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M589" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32096,7 +32093,7 @@
       <c r="J591" s="2"/>
       <c r="K591" s="2"/>
       <c r="L591" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M591" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32130,7 +32127,7 @@
       <c r="J592" s="2"/>
       <c r="K592" s="2"/>
       <c r="L592" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M592" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32198,7 +32195,7 @@
       <c r="J594" s="2"/>
       <c r="K594" s="2"/>
       <c r="L594" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M594" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32232,7 +32229,7 @@
       <c r="J595" s="2"/>
       <c r="K595" s="2"/>
       <c r="L595" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M595" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32300,7 +32297,7 @@
       <c r="J597" s="2"/>
       <c r="K597" s="2"/>
       <c r="L597" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M597" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32334,7 +32331,7 @@
       <c r="J598" s="2"/>
       <c r="K598" s="2"/>
       <c r="L598" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M598" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32402,7 +32399,7 @@
       <c r="J600" s="2"/>
       <c r="K600" s="2"/>
       <c r="L600" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M600" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32436,7 +32433,7 @@
       <c r="J601" s="2"/>
       <c r="K601" s="2"/>
       <c r="L601" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M601" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32504,7 +32501,7 @@
       <c r="J603" s="2"/>
       <c r="K603" s="2"/>
       <c r="L603" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M603" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32538,7 +32535,7 @@
       <c r="J604" s="2"/>
       <c r="K604" s="2"/>
       <c r="L604" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M604" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32606,7 +32603,7 @@
       <c r="J606" s="2"/>
       <c r="K606" s="2"/>
       <c r="L606" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="M606" s="26" t="str">
         <f t="shared" si="9"/>
@@ -32640,7 +32637,7 @@
       <c r="J607" s="2"/>
       <c r="K607" s="2"/>
       <c r="L607" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="M607" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33192,7 +33189,7 @@
       <c r="J624" s="2"/>
       <c r="K624" s="2"/>
       <c r="L624" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M624" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33226,7 +33223,7 @@
       <c r="J625" s="2"/>
       <c r="K625" s="2"/>
       <c r="L625" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M625" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33260,7 +33257,7 @@
       <c r="J626" s="2"/>
       <c r="K626" s="2"/>
       <c r="L626" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M626" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33294,7 +33291,7 @@
       <c r="J627" s="2"/>
       <c r="K627" s="2"/>
       <c r="L627" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M627" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33328,7 +33325,7 @@
       <c r="J628" s="2"/>
       <c r="K628" s="2"/>
       <c r="L628" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M628" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33362,7 +33359,7 @@
       <c r="J629" s="2"/>
       <c r="K629" s="2"/>
       <c r="L629" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M629" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33396,7 +33393,7 @@
       <c r="J630" s="2"/>
       <c r="K630" s="2"/>
       <c r="L630" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M630" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33430,7 +33427,7 @@
       <c r="J631" s="2"/>
       <c r="K631" s="2"/>
       <c r="L631" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M631" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33464,7 +33461,7 @@
       <c r="J632" s="2"/>
       <c r="K632" s="2"/>
       <c r="L632" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M632" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33498,7 +33495,7 @@
       <c r="J633" s="2"/>
       <c r="K633" s="2"/>
       <c r="L633" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M633" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33532,7 +33529,7 @@
       <c r="J634" s="2"/>
       <c r="K634" s="2"/>
       <c r="L634" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M634" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33566,7 +33563,7 @@
       <c r="J635" s="2"/>
       <c r="K635" s="2"/>
       <c r="L635" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M635" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33600,7 +33597,7 @@
       <c r="J636" s="2"/>
       <c r="K636" s="2"/>
       <c r="L636" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M636" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33634,7 +33631,7 @@
       <c r="J637" s="2"/>
       <c r="K637" s="2"/>
       <c r="L637" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M637" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33668,7 +33665,7 @@
       <c r="J638" s="2"/>
       <c r="K638" s="2"/>
       <c r="L638" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M638" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33702,7 +33699,7 @@
       <c r="J639" s="2"/>
       <c r="K639" s="2"/>
       <c r="L639" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M639" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33736,7 +33733,7 @@
       <c r="J640" s="2"/>
       <c r="K640" s="2"/>
       <c r="L640" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M640" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33770,7 +33767,7 @@
       <c r="J641" s="2"/>
       <c r="K641" s="2"/>
       <c r="L641" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M641" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33804,7 +33801,7 @@
       <c r="J642" s="2"/>
       <c r="K642" s="2"/>
       <c r="L642" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M642" s="26" t="str">
         <f t="shared" si="9"/>
@@ -33838,7 +33835,7 @@
       <c r="J643" s="2"/>
       <c r="K643" s="2"/>
       <c r="L643" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M643" s="26" t="str">
         <f t="shared" ref="M643:M706" si="10">IF(C643="Numeric", "number",IF(C643="Date","date",IF(E643="Yes ; No", "boolean","string")))</f>
@@ -33872,7 +33869,7 @@
       <c r="J644" s="2"/>
       <c r="K644" s="2"/>
       <c r="L644" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M644" s="26" t="str">
         <f t="shared" si="10"/>
@@ -33906,7 +33903,7 @@
       <c r="J645" s="2"/>
       <c r="K645" s="2"/>
       <c r="L645" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="M645" s="26" t="str">
         <f t="shared" si="10"/>
@@ -33940,7 +33937,7 @@
       <c r="J646" s="2"/>
       <c r="K646" s="2"/>
       <c r="L646" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="M646" s="26" t="str">
         <f t="shared" si="10"/>
@@ -33974,7 +33971,7 @@
       <c r="J647" s="2"/>
       <c r="K647" s="2"/>
       <c r="L647" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="M647" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34008,7 +34005,7 @@
       <c r="J648" s="2"/>
       <c r="K648" s="2"/>
       <c r="L648" s="2" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="M648" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34044,7 +34041,7 @@
       <c r="J649" s="2"/>
       <c r="K649" s="2"/>
       <c r="L649" s="2" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
       <c r="M649" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34112,7 +34109,7 @@
       <c r="J651" s="2"/>
       <c r="K651" s="2"/>
       <c r="L651" s="2" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="M651" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34148,7 +34145,7 @@
       <c r="J652" s="2"/>
       <c r="K652" s="2"/>
       <c r="L652" s="2" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
       <c r="M652" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34216,7 +34213,7 @@
       <c r="J654" s="2"/>
       <c r="K654" s="2"/>
       <c r="L654" s="2" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="M654" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34252,7 +34249,7 @@
       <c r="J655" s="2"/>
       <c r="K655" s="2"/>
       <c r="L655" s="2" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
       <c r="M655" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34388,7 +34385,7 @@
       <c r="J659" s="2"/>
       <c r="K659" s="2"/>
       <c r="L659" s="2" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="M659" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34422,7 +34419,7 @@
       <c r="J660" s="2"/>
       <c r="K660" s="2"/>
       <c r="L660" s="2" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="M660" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34458,7 +34455,7 @@
       <c r="J661" s="2"/>
       <c r="K661" s="2"/>
       <c r="L661" s="2" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="M661" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34492,7 +34489,7 @@
       <c r="J662" s="2"/>
       <c r="K662" s="2"/>
       <c r="L662" s="2" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="M662" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34526,7 +34523,7 @@
       <c r="J663" s="2"/>
       <c r="K663" s="2"/>
       <c r="L663" s="2" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="M663" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34560,7 +34557,7 @@
       <c r="J664" s="2"/>
       <c r="K664" s="2"/>
       <c r="L664" s="2" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="M664" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34596,7 +34593,7 @@
       <c r="J665" s="2"/>
       <c r="K665" s="2"/>
       <c r="L665" s="2" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="M665" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34630,7 +34627,7 @@
       <c r="J666" s="2"/>
       <c r="K666" s="2"/>
       <c r="L666" s="2" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="M666" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34664,7 +34661,7 @@
       <c r="J667" s="2"/>
       <c r="K667" s="2"/>
       <c r="L667" s="2" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="M667" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34698,7 +34695,7 @@
       <c r="J668" s="2"/>
       <c r="K668" s="2"/>
       <c r="L668" s="2" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="M668" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34734,7 +34731,7 @@
       <c r="J669" s="2"/>
       <c r="K669" s="2"/>
       <c r="L669" s="2" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="M669" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34768,7 +34765,7 @@
       <c r="J670" s="2"/>
       <c r="K670" s="2"/>
       <c r="L670" s="2" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="M670" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34802,7 +34799,7 @@
       <c r="J671" s="2"/>
       <c r="K671" s="2"/>
       <c r="L671" s="2" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="M671" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34836,7 +34833,7 @@
       <c r="J672" s="2"/>
       <c r="K672" s="2"/>
       <c r="L672" s="2" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="M672" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34872,7 +34869,7 @@
       <c r="J673" s="2"/>
       <c r="K673" s="2"/>
       <c r="L673" s="2" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="M673" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34906,7 +34903,7 @@
       <c r="J674" s="2"/>
       <c r="K674" s="2"/>
       <c r="L674" s="2" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="M674" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34942,7 +34939,7 @@
       <c r="J675" s="2"/>
       <c r="K675" s="2"/>
       <c r="L675" s="2" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="M675" s="26" t="str">
         <f t="shared" si="10"/>
@@ -34978,7 +34975,7 @@
       <c r="J676" s="2"/>
       <c r="K676" s="2"/>
       <c r="L676" s="2" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="M676" s="26" t="str">
         <f t="shared" si="10"/>
@@ -35012,7 +35009,7 @@
       <c r="J677" s="2"/>
       <c r="K677" s="2"/>
       <c r="L677" s="2" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="M677" s="26" t="str">
         <f t="shared" si="10"/>
@@ -35116,7 +35113,7 @@
       <c r="J680" s="2"/>
       <c r="K680" s="2"/>
       <c r="L680" s="2" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="M680" s="26" t="str">
         <f t="shared" si="10"/>
@@ -35152,7 +35149,7 @@
       <c r="J681" s="2"/>
       <c r="K681" s="2"/>
       <c r="L681" s="2" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="M681" s="26" t="str">
         <f t="shared" si="10"/>
@@ -35186,7 +35183,7 @@
       <c r="J682" s="2"/>
       <c r="K682" s="2"/>
       <c r="L682" s="2" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="M682" s="26" t="str">
         <f t="shared" si="10"/>
@@ -36372,7 +36369,7 @@
       <c r="J717" s="2"/>
       <c r="K717" s="2"/>
       <c r="L717" s="23" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="M717" s="26" t="str">
         <f t="shared" si="11"/>
@@ -36830,7 +36827,7 @@
       <c r="J731" s="2"/>
       <c r="K731" s="2"/>
       <c r="L731" s="2" t="s">
-        <v>3818</v>
+        <v>3817</v>
       </c>
       <c r="M731" s="26" t="str">
         <f t="shared" si="11"/>
@@ -36862,7 +36859,7 @@
       <c r="J732" s="2"/>
       <c r="K732" s="2"/>
       <c r="L732" s="2" t="s">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="M732" s="26" t="str">
         <f t="shared" si="11"/>
@@ -36960,7 +36957,7 @@
       <c r="J735" s="2"/>
       <c r="K735" s="2"/>
       <c r="L735" s="2" t="s">
-        <v>3820</v>
+        <v>3819</v>
       </c>
       <c r="M735" s="26" t="str">
         <f t="shared" si="11"/>
@@ -46598,7 +46595,7 @@
       <c r="J1003" s="2"/>
       <c r="K1003" s="2"/>
       <c r="L1003" s="2" t="s">
-        <v>3833</v>
+        <v>3832</v>
       </c>
       <c r="M1003" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46628,7 +46625,7 @@
       <c r="J1004" s="2"/>
       <c r="K1004" s="2"/>
       <c r="L1004" s="2" t="s">
-        <v>3832</v>
+        <v>3831</v>
       </c>
       <c r="M1004" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46658,7 +46655,7 @@
       <c r="J1005" s="2"/>
       <c r="K1005" s="2"/>
       <c r="L1005" s="2" t="s">
-        <v>3831</v>
+        <v>3830</v>
       </c>
       <c r="M1005" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46718,7 +46715,7 @@
       <c r="J1007" s="2"/>
       <c r="K1007" s="2"/>
       <c r="L1007" s="2" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="M1007" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46748,7 +46745,7 @@
       <c r="J1008" s="2"/>
       <c r="K1008" s="2"/>
       <c r="L1008" s="2" t="s">
-        <v>3821</v>
+        <v>3820</v>
       </c>
       <c r="M1008" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46778,7 +46775,7 @@
       <c r="J1009" s="2"/>
       <c r="K1009" s="2"/>
       <c r="L1009" s="2" t="s">
-        <v>3822</v>
+        <v>3821</v>
       </c>
       <c r="M1009" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46808,7 +46805,7 @@
       <c r="J1010" s="2"/>
       <c r="K1010" s="2"/>
       <c r="L1010" s="2" t="s">
-        <v>3823</v>
+        <v>3822</v>
       </c>
       <c r="M1010" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46871,7 +46868,7 @@
       <c r="J1012" s="2"/>
       <c r="K1012" s="2"/>
       <c r="L1012" s="2" t="s">
-        <v>3824</v>
+        <v>3823</v>
       </c>
       <c r="M1012" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46901,7 +46898,7 @@
       <c r="J1013" s="2"/>
       <c r="K1013" s="2"/>
       <c r="L1013" s="2" t="s">
-        <v>3825</v>
+        <v>3824</v>
       </c>
       <c r="M1013" s="26" t="str">
         <f t="shared" si="15"/>
@@ -46931,7 +46928,7 @@
       <c r="J1014" s="2"/>
       <c r="K1014" s="2"/>
       <c r="L1014" s="2" t="s">
-        <v>3826</v>
+        <v>3825</v>
       </c>
       <c r="M1014" s="26" t="str">
         <f t="shared" si="15"/>
@@ -47051,7 +47048,7 @@
       <c r="J1018" s="2"/>
       <c r="K1018" s="2"/>
       <c r="L1018" s="2" t="s">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="M1018" s="26" t="str">
         <f t="shared" si="15"/>
@@ -47081,7 +47078,7 @@
       <c r="J1019" s="2"/>
       <c r="K1019" s="2"/>
       <c r="L1019" s="2" t="s">
-        <v>3828</v>
+        <v>3827</v>
       </c>
       <c r="M1019" s="26" t="str">
         <f t="shared" si="15"/>
@@ -47111,7 +47108,7 @@
       <c r="J1020" s="2"/>
       <c r="K1020" s="2"/>
       <c r="L1020" s="2" t="s">
-        <v>3829</v>
+        <v>3828</v>
       </c>
       <c r="M1020" s="26" t="str">
         <f t="shared" si="15"/>
@@ -47141,7 +47138,7 @@
       <c r="J1021" s="2"/>
       <c r="K1021" s="2"/>
       <c r="L1021" s="2" t="s">
-        <v>3830</v>
+        <v>3829</v>
       </c>
       <c r="M1021" s="26" t="str">
         <f t="shared" si="15"/>

</xml_diff>